<commit_message>
ready for second recruiting session
</commit_message>
<xml_diff>
--- a/candidates.xlsx
+++ b/candidates.xlsx
@@ -1,78 +1,58 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\enactus\matching_enactus_munich\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B096B72-CB46-41AB-8737-ACD126A6EEC6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="EduGlobe" sheetId="1" r:id="rId1"/>
+    <sheet name="FoodGrube" sheetId="2" r:id="rId2"/>
+    <sheet name="Mistub" sheetId="3" r:id="rId3"/>
+    <sheet name="SeaSoilution" sheetId="4" r:id="rId4"/>
+    <sheet name="TownBee" sheetId="5" r:id="rId5"/>
+    <sheet name="Operations" sheetId="6" r:id="rId6"/>
+    <sheet name="ReStove" sheetId="7" r:id="rId7"/>
+    <sheet name="Waterfilter" sheetId="8" r:id="rId8"/>
+    <sheet name="Glassic" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
   <si>
-    <t>EduGlobe</t>
+    <t>Vorname</t>
   </si>
   <si>
-    <t>Foodgrube</t>
+    <t>Prio</t>
   </si>
   <si>
-    <t>Mistub</t>
+    <t>Hallo Ich bin Test</t>
   </si>
   <si>
-    <t>SeaSoilution</t>
+    <t>Prio 3</t>
   </si>
   <si>
-    <t>Townbee</t>
-  </si>
-  <si>
-    <t>Operations</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>I</t>
+    <t>Prio 4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -88,7 +68,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -96,26 +76,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -162,7 +152,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -194,27 +184,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -246,24 +218,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -439,112 +393,149 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C2" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="D6" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>